<commit_message>
Changes Committed to report and updated data
</commit_message>
<xml_diff>
--- a/2023_forecast/data/f_model_one_step_ahead function check.xlsx
+++ b/2023_forecast/data/f_model_one_step_ahead function check.xlsx
@@ -1,20 +1,29 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="25427"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="25629"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\preseason_SEAK_pink_salmon_forecast\2023_forecast\data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4CB68FA2-703E-4D99-A2CE-1E2430E847DD}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9D54D31C-24E1-43FB-8B76-D7F64BED440E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="f_model_one_step_ahead function" sheetId="1" r:id="rId1"/>
   </sheets>
+  <definedNames>
+    <definedName name="solver_eng" localSheetId="0" hidden="1">1</definedName>
+    <definedName name="solver_neg" localSheetId="0" hidden="1">1</definedName>
+    <definedName name="solver_num" localSheetId="0" hidden="1">0</definedName>
+    <definedName name="solver_opt" localSheetId="0" hidden="1">'f_model_one_step_ahead function'!$I$4</definedName>
+    <definedName name="solver_typ" localSheetId="0" hidden="1">1</definedName>
+    <definedName name="solver_val" localSheetId="0" hidden="1">0</definedName>
+    <definedName name="solver_ver" localSheetId="0" hidden="1">3</definedName>
+  </definedNames>
   <calcPr calcId="191029"/>
   <extLst>
     <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
@@ -32,7 +41,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="57" uniqueCount="54">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="71" uniqueCount="65">
   <si>
     <t>JYear</t>
   </si>
@@ -194,6 +203,39 @@
   </si>
   <si>
     <t>exp(obs)</t>
+  </si>
+  <si>
+    <t>model</t>
+  </si>
+  <si>
+    <t>term</t>
+  </si>
+  <si>
+    <t>estimate</t>
+  </si>
+  <si>
+    <t>std.error</t>
+  </si>
+  <si>
+    <t>statistic</t>
+  </si>
+  <si>
+    <t>p.value</t>
+  </si>
+  <si>
+    <t>(Intercept)</t>
+  </si>
+  <si>
+    <t>CPUE</t>
+  </si>
+  <si>
+    <t>m11</t>
+  </si>
+  <si>
+    <t>sigma</t>
+  </si>
+  <si>
+    <t>best  model</t>
   </si>
 </sst>
 </file>
@@ -711,19 +753,17 @@
     <xf numFmtId="0" fontId="1" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="1" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="8">
+  <cellXfs count="6">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="33" borderId="0" xfId="0" applyFill="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="18" fillId="0" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="18" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="18" fillId="0" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="18" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="centerContinuous"/>
     </xf>
   </cellXfs>
@@ -1083,12 +1123,15 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:AE47"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="L1" workbookViewId="0">
-      <selection activeCell="AH30" sqref="AH30"/>
+    <sheetView tabSelected="1" topLeftCell="E1" workbookViewId="0">
+      <selection activeCell="P34" sqref="P34"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
+    <col min="13" max="13" width="15.140625" bestFit="1" customWidth="1"/>
+    <col min="14" max="14" width="15.7109375" bestFit="1" customWidth="1"/>
+    <col min="16" max="16" width="15.7109375" bestFit="1" customWidth="1"/>
     <col min="23" max="23" width="14" bestFit="1" customWidth="1"/>
     <col min="29" max="29" width="12.42578125" bestFit="1" customWidth="1"/>
   </cols>
@@ -2756,7 +2799,7 @@
       <c r="W22">
         <v>1</v>
       </c>
-      <c r="X22" s="3">
+      <c r="X22">
         <f>LN(C22)</f>
         <v>2.0918640616783932</v>
       </c>
@@ -2780,7 +2823,7 @@
         <v>0.77661522014079809</v>
       </c>
       <c r="AE22">
-        <f>AVERAGE(ABS((X22-AA22)/X22))</f>
+        <f>(ABS((X22-AA22)/X22))</f>
         <v>0.27473582191592882</v>
       </c>
     </row>
@@ -2854,8 +2897,8 @@
       <c r="W23">
         <v>1</v>
       </c>
-      <c r="X23" s="3">
-        <f t="shared" ref="X3:X26" si="1">LN(C23)</f>
+      <c r="X23">
+        <f t="shared" ref="X23:X25" si="1">LN(C23)</f>
         <v>3.0492730404820207</v>
       </c>
       <c r="AA23" s="1">
@@ -2874,7 +2917,7 @@
         <v>0.17146599962300355</v>
       </c>
       <c r="AE23">
-        <f>AVERAGE(ABS((X23-AA23)/X23))</f>
+        <f>(ABS((X23-AA23)/X23))</f>
         <v>6.1685982850616355E-2</v>
       </c>
     </row>
@@ -2948,7 +2991,7 @@
       <c r="W24">
         <v>1</v>
       </c>
-      <c r="X24" s="3">
+      <c r="X24">
         <f t="shared" si="1"/>
         <v>2.0878985551190659</v>
       </c>
@@ -2968,7 +3011,7 @@
         <v>1.1901079785368971</v>
       </c>
       <c r="AE24">
-        <f>AVERAGE(ABS((X24-AA24)/X24))</f>
+        <f t="shared" ref="AE24:AE26" si="3">(ABS((X24-AA24)/X24))</f>
         <v>0.37547362919470395</v>
       </c>
     </row>
@@ -3042,7 +3085,7 @@
       <c r="W25">
         <v>1</v>
       </c>
-      <c r="X25" s="3">
+      <c r="X25">
         <f t="shared" si="1"/>
         <v>3.8794998137225858</v>
       </c>
@@ -3062,7 +3105,7 @@
         <v>0.47865506957026582</v>
       </c>
       <c r="AE25">
-        <f>AVERAGE(ABS((X25-AA25)/X25))</f>
+        <f t="shared" si="3"/>
         <v>0.16789365459398931</v>
       </c>
     </row>
@@ -3074,7 +3117,7 @@
         <v>2022</v>
       </c>
       <c r="C26">
-        <v>16</v>
+        <v>18.036332000000002</v>
       </c>
       <c r="D26">
         <v>8.8855099210000006</v>
@@ -3136,9 +3179,9 @@
       <c r="W26">
         <v>1</v>
       </c>
-      <c r="X26" s="3">
-        <f t="shared" si="1"/>
-        <v>2.7725887222397811</v>
+      <c r="X26">
+        <f>LN(C26)</f>
+        <v>2.8923881680186057</v>
       </c>
       <c r="AA26" s="1">
         <v>2.7121490000000001</v>
@@ -3149,15 +3192,15 @@
       </c>
       <c r="AC26">
         <f>EXP(X26)</f>
-        <v>15.999999999999998</v>
+        <v>18.036332000000002</v>
       </c>
       <c r="AD26">
         <f t="shared" si="2"/>
-        <v>5.8649490191403093E-2</v>
+        <v>0.1649295346228076</v>
       </c>
       <c r="AE26">
-        <f>AVERAGE(ABS((X26-AA26)/X26))</f>
-        <v>2.179902188700961E-2</v>
+        <f t="shared" si="3"/>
+        <v>6.2314999767847927E-2</v>
       </c>
     </row>
     <row r="27" spans="1:31" x14ac:dyDescent="0.25">
@@ -3234,11 +3277,11 @@
     <row r="29" spans="1:31" x14ac:dyDescent="0.25">
       <c r="AD29">
         <f>AVERAGE(AD22:AD26)</f>
-        <v>0.53509875161247344</v>
+        <v>0.55635476049875443</v>
       </c>
       <c r="AE29">
         <f>AVERAGE(AE22:AE26)</f>
-        <v>0.18031762208844962</v>
+        <v>0.18842081766461727</v>
       </c>
     </row>
     <row r="30" spans="1:31" x14ac:dyDescent="0.25">
@@ -3248,207 +3291,294 @@
     </row>
     <row r="31" spans="1:31" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
     <row r="32" spans="1:31" x14ac:dyDescent="0.25">
-      <c r="F32" s="7" t="s">
+      <c r="F32" s="5" t="s">
         <v>25</v>
       </c>
-      <c r="G32" s="7"/>
-    </row>
-    <row r="33" spans="6:14" x14ac:dyDescent="0.25">
-      <c r="F33" s="4" t="s">
+      <c r="G32" s="5"/>
+    </row>
+    <row r="33" spans="6:27" x14ac:dyDescent="0.25">
+      <c r="F33" t="s">
         <v>26</v>
       </c>
-      <c r="G33" s="4">
+      <c r="G33">
         <v>0.72276230532566521</v>
       </c>
-    </row>
-    <row r="34" spans="6:14" x14ac:dyDescent="0.25">
-      <c r="F34" s="4" t="s">
+      <c r="S33" t="s">
+        <v>64</v>
+      </c>
+    </row>
+    <row r="34" spans="6:27" x14ac:dyDescent="0.25">
+      <c r="F34" t="s">
         <v>27</v>
       </c>
-      <c r="G34" s="4">
+      <c r="G34">
         <v>0.52238534999967012</v>
       </c>
-    </row>
-    <row r="35" spans="6:14" x14ac:dyDescent="0.25">
-      <c r="F35" s="4" t="s">
+      <c r="S34" t="s">
+        <v>54</v>
+      </c>
+      <c r="T34" t="s">
+        <v>55</v>
+      </c>
+      <c r="U34" t="s">
+        <v>56</v>
+      </c>
+      <c r="V34" t="s">
+        <v>57</v>
+      </c>
+      <c r="W34" t="s">
+        <v>58</v>
+      </c>
+      <c r="X34" t="s">
+        <v>59</v>
+      </c>
+      <c r="Y34" t="s">
+        <v>63</v>
+      </c>
+    </row>
+    <row r="35" spans="6:27" x14ac:dyDescent="0.25">
+      <c r="F35" t="s">
         <v>28</v>
       </c>
-      <c r="G35" s="4">
+      <c r="G35">
         <v>0.49585120277742956</v>
       </c>
-    </row>
-    <row r="36" spans="6:14" x14ac:dyDescent="0.25">
-      <c r="F36" s="4" t="s">
+      <c r="S35" t="s">
+        <v>62</v>
+      </c>
+      <c r="T35" t="s">
+        <v>60</v>
+      </c>
+      <c r="U35">
+        <v>5.2720784700000003</v>
+      </c>
+      <c r="V35">
+        <v>0.67</v>
+      </c>
+      <c r="W35">
+        <v>7.8710000000000004</v>
+      </c>
+      <c r="X35">
+        <v>0</v>
+      </c>
+      <c r="Y35">
+        <v>0.31222536789385502</v>
+      </c>
+      <c r="Z35">
+        <f>U35+(U36*V27)+(U37*N27)</f>
+        <v>2.8857583594323017</v>
+      </c>
+      <c r="AA35">
+        <f>EXP(Z35)*EXP(0.5*Y35*Y35)</f>
+        <v>18.812107897057018</v>
+      </c>
+    </row>
+    <row r="36" spans="6:27" x14ac:dyDescent="0.25">
+      <c r="F36" t="s">
         <v>29</v>
       </c>
-      <c r="G36" s="4">
+      <c r="G36">
         <v>0.39534780441303374</v>
       </c>
-    </row>
-    <row r="37" spans="6:14" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="F37" s="5" t="s">
+      <c r="S36" t="s">
+        <v>62</v>
+      </c>
+      <c r="T36" t="s">
+        <v>61</v>
+      </c>
+      <c r="U36">
+        <v>0.45925796000000002</v>
+      </c>
+      <c r="V36">
+        <v>5.1999999999999998E-2</v>
+      </c>
+      <c r="W36">
+        <v>8.8789999999999996</v>
+      </c>
+      <c r="X36">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="37" spans="6:27" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="F37" s="3" t="s">
         <v>30</v>
       </c>
-      <c r="G37" s="5">
+      <c r="G37" s="3">
         <v>20</v>
       </c>
-    </row>
-    <row r="39" spans="6:14" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="S37" t="s">
+        <v>62</v>
+      </c>
+      <c r="T37" t="s">
+        <v>13</v>
+      </c>
+      <c r="U37">
+        <v>-0.40041544000000001</v>
+      </c>
+      <c r="V37">
+        <v>0.09</v>
+      </c>
+      <c r="W37">
+        <v>-4.4489999999999998</v>
+      </c>
+      <c r="X37">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="39" spans="6:27" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="F39" t="s">
         <v>31</v>
       </c>
     </row>
-    <row r="40" spans="6:14" x14ac:dyDescent="0.25">
-      <c r="F40" s="6"/>
-      <c r="G40" s="6" t="s">
+    <row r="40" spans="6:27" x14ac:dyDescent="0.25">
+      <c r="F40" s="4"/>
+      <c r="G40" s="4" t="s">
         <v>32</v>
       </c>
-      <c r="H40" s="6" t="s">
+      <c r="H40" s="4" t="s">
         <v>33</v>
       </c>
-      <c r="I40" s="6" t="s">
+      <c r="I40" s="4" t="s">
         <v>34</v>
       </c>
-      <c r="J40" s="6" t="s">
+      <c r="J40" s="4" t="s">
         <v>35</v>
       </c>
-      <c r="K40" s="6" t="s">
+      <c r="K40" s="4" t="s">
         <v>36</v>
       </c>
     </row>
-    <row r="41" spans="6:14" x14ac:dyDescent="0.25">
-      <c r="F41" s="4" t="s">
+    <row r="41" spans="6:27" x14ac:dyDescent="0.25">
+      <c r="F41" t="s">
         <v>37</v>
       </c>
-      <c r="G41" s="4">
+      <c r="G41">
         <v>1</v>
       </c>
-      <c r="H41" s="4">
+      <c r="H41">
         <v>3.0771205950742764</v>
       </c>
-      <c r="I41" s="4">
+      <c r="I41">
         <v>3.0771205950742764</v>
       </c>
-      <c r="J41" s="4">
+      <c r="J41">
         <v>19.687286183511262</v>
       </c>
-      <c r="K41" s="4">
+      <c r="K41">
         <v>3.1830644227253871E-4</v>
       </c>
     </row>
-    <row r="42" spans="6:14" x14ac:dyDescent="0.25">
-      <c r="F42" s="4" t="s">
+    <row r="42" spans="6:27" x14ac:dyDescent="0.25">
+      <c r="F42" t="s">
         <v>38</v>
       </c>
-      <c r="G42" s="4">
+      <c r="G42">
         <v>18</v>
       </c>
-      <c r="H42" s="4">
+      <c r="H42">
         <v>2.8133979561757152</v>
       </c>
-      <c r="I42" s="4">
+      <c r="I42">
         <v>0.15629988645420639</v>
       </c>
-      <c r="J42" s="4"/>
-      <c r="K42" s="4"/>
-    </row>
-    <row r="43" spans="6:14" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="F43" s="5" t="s">
+    </row>
+    <row r="43" spans="6:27" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="F43" s="3" t="s">
         <v>39</v>
       </c>
-      <c r="G43" s="5">
+      <c r="G43" s="3">
         <v>19</v>
       </c>
-      <c r="H43" s="5">
+      <c r="H43" s="3">
         <v>5.8905185512499916</v>
       </c>
-      <c r="I43" s="5"/>
-      <c r="J43" s="5"/>
-      <c r="K43" s="5"/>
-    </row>
-    <row r="44" spans="6:14" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
-    <row r="45" spans="6:14" x14ac:dyDescent="0.25">
-      <c r="F45" s="6"/>
-      <c r="G45" s="6" t="s">
+      <c r="I43" s="3"/>
+      <c r="J43" s="3"/>
+      <c r="K43" s="3"/>
+    </row>
+    <row r="44" spans="6:27" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
+    <row r="45" spans="6:27" x14ac:dyDescent="0.25">
+      <c r="F45" s="4"/>
+      <c r="G45" s="4" t="s">
         <v>40</v>
       </c>
-      <c r="H45" s="6" t="s">
+      <c r="H45" s="4" t="s">
         <v>29</v>
       </c>
-      <c r="I45" s="6" t="s">
+      <c r="I45" s="4" t="s">
         <v>41</v>
       </c>
-      <c r="J45" s="6" t="s">
+      <c r="J45" s="4" t="s">
         <v>42</v>
       </c>
-      <c r="K45" s="6" t="s">
+      <c r="K45" s="4" t="s">
         <v>43</v>
       </c>
-      <c r="L45" s="6" t="s">
+      <c r="L45" s="4" t="s">
         <v>44</v>
       </c>
-      <c r="M45" s="6" t="s">
+      <c r="M45" s="4" t="s">
         <v>45</v>
       </c>
-      <c r="N45" s="6" t="s">
+      <c r="N45" s="4" t="s">
         <v>46</v>
       </c>
     </row>
-    <row r="46" spans="6:14" x14ac:dyDescent="0.25">
-      <c r="F46" s="4" t="s">
+    <row r="46" spans="6:27" x14ac:dyDescent="0.25">
+      <c r="F46" t="s">
         <v>47</v>
       </c>
-      <c r="G46" s="4">
+      <c r="G46">
         <v>2.5384529992175402</v>
       </c>
-      <c r="H46" s="4">
+      <c r="H46">
         <v>0.25653372929530588</v>
       </c>
-      <c r="I46" s="4">
+      <c r="I46">
         <v>9.8952017194410686</v>
       </c>
-      <c r="J46" s="4">
+      <c r="J46">
         <v>1.0500316902262048E-8</v>
       </c>
-      <c r="K46" s="4">
+      <c r="K46">
         <v>1.999495633275804</v>
       </c>
-      <c r="L46" s="4">
+      <c r="L46">
         <v>3.0774103651592766</v>
       </c>
-      <c r="M46" s="4">
+      <c r="M46">
         <v>1.999495633275804</v>
       </c>
-      <c r="N46" s="4">
+      <c r="N46">
         <v>3.0774103651592766</v>
       </c>
     </row>
-    <row r="47" spans="6:14" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="F47" s="5" t="s">
+    <row r="47" spans="6:27" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="F47" s="3" t="s">
         <v>48</v>
       </c>
-      <c r="G47" s="5">
+      <c r="G47" s="3">
         <v>0.3660601564047215</v>
       </c>
-      <c r="H47" s="5">
+      <c r="H47" s="3">
         <v>8.250106098264022E-2</v>
       </c>
-      <c r="I47" s="5">
+      <c r="I47" s="3">
         <v>4.4370357428705978</v>
       </c>
-      <c r="J47" s="5">
+      <c r="J47" s="3">
         <v>3.183064422725411E-4</v>
       </c>
-      <c r="K47" s="5">
+      <c r="K47" s="3">
         <v>0.19273185904302273</v>
       </c>
-      <c r="L47" s="5">
+      <c r="L47" s="3">
         <v>0.53938845376642031</v>
       </c>
-      <c r="M47" s="5">
+      <c r="M47" s="3">
         <v>0.19273185904302273</v>
       </c>
-      <c r="N47" s="5">
+      <c r="N47" s="3">
         <v>0.53938845376642031</v>
       </c>
     </row>

</xml_diff>